<commit_message>
reordered model training file
</commit_message>
<xml_diff>
--- a/SOL_Index_by_Country.xlsx
+++ b/SOL_Index_by_Country.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
readjusted comments and format
</commit_message>
<xml_diff>
--- a/SOL_Index_by_Country.xlsx
+++ b/SOL_Index_by_Country.xlsx
@@ -550,7 +550,7 @@
         <v>29.43809527442569</v>
       </c>
       <c r="H2" t="n">
-        <v>89.96190476190476</v>
+        <v>33097480.50891428</v>
       </c>
       <c r="I2" t="n">
         <v>90.47619047619048</v>
@@ -574,13 +574,13 @@
         <v>0.2943809527442569</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8996190476190477</v>
+        <v>1</v>
       </c>
       <c r="Q2" t="n">
         <v>0.9047619047619048</v>
       </c>
       <c r="R2" t="n">
-        <v>0.8629214920557889</v>
+        <v>0.8684982116325085</v>
       </c>
     </row>
     <row r="3">
@@ -608,7 +608,7 @@
         <v>17.9238099143619</v>
       </c>
       <c r="H3" t="n">
-        <v>86.01904761904763</v>
+        <v>13199084.11926667</v>
       </c>
       <c r="I3" t="n">
         <v>91.42857142857143</v>
@@ -632,13 +632,13 @@
         <v>0.179238099143619</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8601904761904763</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="n">
         <v>0.9142857142857143</v>
       </c>
       <c r="R3" t="n">
-        <v>0.789249002172414</v>
+        <v>0.7970161979396098</v>
       </c>
     </row>
     <row r="4">
@@ -666,7 +666,7 @@
         <v>13.31904729207359</v>
       </c>
       <c r="H4" t="n">
-        <v>71.96190476190476</v>
+        <v>28686217.44162857</v>
       </c>
       <c r="I4" t="n">
         <v>71.71428571428571</v>
@@ -690,13 +690,13 @@
         <v>0.1331904729207359</v>
       </c>
       <c r="P4" t="n">
-        <v>0.7196190476190476</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="n">
         <v>0.7171428571428571</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7096039085944646</v>
+        <v>0.7251806281711842</v>
       </c>
     </row>
     <row r="5">
@@ -724,7 +724,7 @@
         <v>54.02655205654723</v>
       </c>
       <c r="H5" t="n">
-        <v>41.97142857142857</v>
+        <v>90637424.57813333</v>
       </c>
       <c r="I5" t="n">
         <v>43.47619047619047</v>
@@ -748,13 +748,13 @@
         <v>0.5402655205654723</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4197142857142857</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="n">
         <v>0.4347619047619047</v>
       </c>
       <c r="R5" t="n">
-        <v>0.5972243196460071</v>
+        <v>0.6294624148841024</v>
       </c>
     </row>
     <row r="6">
@@ -782,7 +782,7 @@
         <v>50.29866592883044</v>
       </c>
       <c r="H6" t="n">
-        <v>27.70476190476192</v>
+        <v>282036016.0624856</v>
       </c>
       <c r="I6" t="n">
         <v>24.76190476190476</v>
@@ -806,13 +806,13 @@
         <v>0.5029866592883043</v>
       </c>
       <c r="P6" t="n">
-        <v>0.2770476190476192</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
         <v>0.2476190476190476</v>
       </c>
       <c r="R6" t="n">
-        <v>0.4780283983067622</v>
+        <v>0.5181924194707834</v>
       </c>
     </row>
     <row r="7">
@@ -840,7 +840,7 @@
         <v>34.07476159596003</v>
       </c>
       <c r="H7" t="n">
-        <v>74.74285714285713</v>
+        <v>74453929.92138095</v>
       </c>
       <c r="I7" t="n">
         <v>76.47619047619048</v>
@@ -864,13 +864,13 @@
         <v>0.3407476159596003</v>
       </c>
       <c r="P7" t="n">
-        <v>0.7474285714285713</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
         <v>0.7647619047619049</v>
       </c>
       <c r="R7" t="n">
-        <v>0.7764096422872296</v>
+        <v>0.7904413883189757</v>
       </c>
     </row>
     <row r="8">
@@ -898,7 +898,7 @@
         <v>77.49725249236839</v>
       </c>
       <c r="H8" t="n">
-        <v>61.54761904761905</v>
+        <v>14611731.60026667</v>
       </c>
       <c r="I8" t="n">
         <v>91.42857142857143</v>
@@ -922,13 +922,13 @@
         <v>0.7749725249236838</v>
       </c>
       <c r="P8" t="n">
-        <v>0.6154761904761905</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
         <v>0.9142857142857143</v>
       </c>
       <c r="R8" t="n">
-        <v>0.8258803056055768</v>
+        <v>0.8472427394680107</v>
       </c>
     </row>
     <row r="9">
@@ -956,7 +956,7 @@
         <v>66.41885854385322</v>
       </c>
       <c r="H9" t="n">
-        <v>61.47619047619047</v>
+        <v>23569573.22388572</v>
       </c>
       <c r="I9" t="n">
         <v>90</v>
@@ -980,13 +980,13 @@
         <v>0.6641885854385322</v>
       </c>
       <c r="P9" t="n">
-        <v>0.6147619047619047</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="n">
         <v>0.9</v>
       </c>
       <c r="R9" t="n">
-        <v>0.8753623389443856</v>
+        <v>0.8967644553465021</v>
       </c>
     </row>
     <row r="10">
@@ -1014,7 +1014,7 @@
         <v>43.29523831321981</v>
       </c>
       <c r="H10" t="n">
-        <v>53.78095238095239</v>
+        <v>11945368.24797143</v>
       </c>
       <c r="I10" t="n">
         <v>71.85714285714286</v>
@@ -1038,13 +1038,13 @@
         <v>0.432952383132198</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5378095238095238</v>
+        <v>1</v>
       </c>
       <c r="Q10" t="n">
         <v>0.7185714285714286</v>
       </c>
       <c r="R10" t="n">
-        <v>0.7747495029858101</v>
+        <v>0.8004267516630589</v>
       </c>
     </row>
     <row r="11">
@@ -1072,7 +1072,7 @@
         <v>29.71428571428572</v>
       </c>
       <c r="H11" t="n">
-        <v>64.61428571428571</v>
+        <v>41219995.53006667</v>
       </c>
       <c r="I11" t="n">
         <v>87.04761904761905</v>
@@ -1096,13 +1096,13 @@
         <v>0.2971428571428572</v>
       </c>
       <c r="P11" t="n">
-        <v>0.6461428571428571</v>
+        <v>1</v>
       </c>
       <c r="Q11" t="n">
         <v>0.8704761904761905</v>
       </c>
       <c r="R11" t="n">
-        <v>0.7192915364926672</v>
+        <v>0.7389502666513974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>